<commit_message>
material and salary titles
</commit_message>
<xml_diff>
--- a/files/excel/material_Object1.xlsx
+++ b/files/excel/material_Object1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,6 +590,46 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Oxak</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>кг</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>суммы</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Shakhzod</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
create materials and salaries in site, check value is int
</commit_message>
<xml_diff>
--- a/files/excel/material_Object1.xlsx
+++ b/files/excel/material_Object1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,6 +470,166 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Oxak</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>кг</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>доллары</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>effrfwwpkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Sjsnisb</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>кг</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>суммы</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>effrfwwpkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>111111111</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>суммы</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>effrfwwpkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>22222222</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>кг</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>суммы</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>effrfwwpkp</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
create material, salary as manager
</commit_message>
<xml_diff>
--- a/files/excel/material_Object1.xlsx
+++ b/files/excel/material_Object1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>Прораб</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Дата</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -476,7 +481,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Oxak</t>
+          <t>Sjsnisb</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,27 +491,32 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>суммы</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>12</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>доллары</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>60</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>effrfwwpkp</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>22.04.2021</t>
         </is>
       </c>
     </row>
@@ -516,17 +526,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sjsnisb</t>
+          <t>fgrgrg</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>кг</t>
+          <t>м^2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -536,17 +546,22 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>12</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>effrfwwpkp</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>22.04.2021</t>
         </is>
       </c>
     </row>
@@ -556,12 +571,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>111111111</t>
+          <t>122122112</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>kg</t>
+          <t>м</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -576,12 +591,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>80</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>80</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -589,44 +604,9 @@
           <t>effrfwwpkp</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>22222222</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>кг</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>суммы</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>effrfwwpkp</t>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>22.04.2021</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
type in salary and material
</commit_message>
<xml_diff>
--- a/files/excel/material_Object1.xlsx
+++ b/files/excel/material_Object1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,17 +481,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sjsnisb</t>
+          <t>Ehhd</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>кг</t>
+          <t>м^3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>88</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -501,12 +501,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>528</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>22.04.2021</t>
+          <t>24.04.2021</t>
         </is>
       </c>
     </row>
@@ -526,17 +526,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>fgrgrg</t>
+          <t>fwe</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>м^2</t>
+          <t>кг</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -546,12 +546,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>400</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>400</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -561,52 +561,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>22.04.2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>122122112</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>м</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>суммы</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>80</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>effrfwwpkp</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>22.04.2021</t>
+          <t>26.04.2021</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
+ balance after deleting material
</commit_message>
<xml_diff>
--- a/files/excel/material_Object1.xlsx
+++ b/files/excel/material_Object1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,7 +521,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>fwe</t>
+          <t>ttttt</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -536,17 +536,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>400.0</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -561,12 +561,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ttttt</t>
+          <t>Material1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>кг</t>
+          <t>м</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -576,12 +576,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>26.04.2021</t>
+          <t>01.05.2021</t>
         </is>
       </c>
     </row>
@@ -601,12 +601,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Material1</t>
+          <t>material2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>м</t>
+          <t>кг</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -616,12 +616,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>50.0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>material2</t>
+          <t>rfreuwgfpslw</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -656,12 +656,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>50.0</t>
+          <t>5000.0</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>01.05.2021</t>
+          <t>17.05.2021</t>
         </is>
       </c>
     </row>
@@ -681,161 +681,281 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>material3</t>
+          <t>dedede</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>м^3</t>
+          <t>кг</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>5000.0</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>17.05.2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>wdwdw</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>м</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>50.0</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>01.05.2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>5000</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>588.0</t>
+          <t>5000.0</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>450.0</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>17.05.2021</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="A9" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>frfewrf</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>м</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>17.05.2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>kjgrguregfiuesas</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>кг</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>18.05.2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>15588.0</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>10000.0</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>0.0588</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>$450.0588</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>1.5588</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>$8.5588</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>

</xml_diff>